<commit_message>
The following have been changed: FINM3403/tutorials/PracticeMCQ_and_Solns (1).pdf FINM3406/course content/FINM 3406  Tute 2.pptx FINM3406/course content/FINM 3406 Tute 1.pptx FINM3406/course content/FINM 3406 Tute 3.pptx FINM3403/docs/midsemcalculator.xlsx FINM3403/notes/lecture2.md FINM3403/notes/revisionLecture1.md FINM3403/notes/revisionLecture2.md FINM3406/docs/Lecture4.html FINM3406/docs/lecture2.html FINM3406/docs/lecture3.html FINM3406/docs/tutorial1.html FINM3406/docs/tutorial2.html FINM3406/docs/tutorial3.html FINM3406/docs/tutorial4.html FINM3406/notes/lecture2.md FINM3406/notes/lecture3.md FINM3406/notes/lecture4.md FINM3406/notes/tutorial1.md FINM3406/notes/tutorial2.md FINM3406/notes/tutorial3.md FINM3406/notes/tutorial3r2.md FINM3406/notes/tutorial4.md
</commit_message>
<xml_diff>
--- a/FINM3403/docs/midsemcalculator.xlsx
+++ b/FINM3403/docs/midsemcalculator.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22980" windowHeight="5820" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22980" windowHeight="5820"/>
   </bookViews>
   <sheets>
     <sheet name="Topic 1 calculators" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="39">
   <si>
     <t>Bid</t>
   </si>
@@ -42,15 +42,9 @@
     <t>AUD</t>
   </si>
   <si>
-    <t>Yen</t>
-  </si>
-  <si>
     <t>GBP</t>
   </si>
   <si>
-    <t>USD</t>
-  </si>
-  <si>
     <t>Currency 1</t>
   </si>
   <si>
@@ -145,6 +139,9 @@
   </si>
   <si>
     <t>CA = Capital Account + Financial Account + errors and omissions + official reserve account</t>
+  </si>
+  <si>
+    <t>EURO</t>
   </si>
 </sst>
 </file>
@@ -152,7 +149,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -439,10 +436,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -482,27 +478,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -515,6 +505,13 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -797,8 +794,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -807,7 +804,7 @@
     <col min="3" max="3" width="2.140625" customWidth="1"/>
     <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" customWidth="1"/>
-    <col min="9" max="9" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.42578125" customWidth="1"/>
     <col min="10" max="10" width="16.42578125" customWidth="1"/>
     <col min="11" max="11" width="11.140625" customWidth="1"/>
     <col min="12" max="12" width="11.85546875" customWidth="1"/>
@@ -815,32 +812,32 @@
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="12"/>
+      <c r="D2" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="12" t="s">
+      <c r="K2" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="J2" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="K2" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="L2" s="32" t="s">
+      <c r="L2" s="31" t="s">
         <v>1</v>
       </c>
     </row>
@@ -849,39 +846,39 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E3" s="6">
-        <v>0.48759999999999998</v>
-      </c>
-      <c r="F3" s="7">
-        <v>0.48849999999999999</v>
-      </c>
-      <c r="H3" s="20" t="str">
+        <v>1.7395</v>
+      </c>
+      <c r="F3" s="6">
+        <v>1.7395</v>
+      </c>
+      <c r="H3" s="19" t="str">
         <f>IF(D3=D4,"BAD","OK")</f>
-        <v>BAD</v>
-      </c>
-      <c r="I3" s="21" t="str">
+        <v>OK</v>
+      </c>
+      <c r="I3" s="20" t="str">
         <f>CONCATENATE(B3, "/",D3, "  x ", B4, "/", D4)</f>
-        <v>GBP/AUD  x USD/AUD</v>
-      </c>
-      <c r="J3" s="30" t="str">
+        <v>AUD/GBP  x EURO/AUD</v>
+      </c>
+      <c r="J3" s="29" t="str">
         <f>IF(H3="BAD","",CONCATENATE(B3,"/",D4))</f>
-        <v/>
-      </c>
-      <c r="K3" s="21">
+        <v>AUD/AUD</v>
+      </c>
+      <c r="K3" s="20">
         <f>E3*E4</f>
-        <v>0.33498120000000003</v>
-      </c>
-      <c r="L3" s="22">
+        <v>1.4625716</v>
+      </c>
+      <c r="L3" s="21">
         <f>F3*F4</f>
-        <v>0.33603914999999995</v>
+        <v>1.4625716</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -889,39 +886,39 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E4" s="6">
-        <v>0.68700000000000006</v>
-      </c>
-      <c r="F4" s="7">
-        <v>0.68789999999999996</v>
-      </c>
-      <c r="H4" s="23" t="str">
+        <v>0.84079999999999999</v>
+      </c>
+      <c r="F4" s="61">
+        <v>0.84079999999999999</v>
+      </c>
+      <c r="H4" s="22" t="str">
         <f>IF(D3&lt;&gt;D4,"BAD","OK")</f>
-        <v>OK</v>
-      </c>
-      <c r="I4" s="24" t="str">
+        <v>BAD</v>
+      </c>
+      <c r="I4" s="23" t="str">
         <f>CONCATENATE(B3, "/",D3, "  / ", B4, "/", D4)</f>
-        <v>GBP/AUD  / USD/AUD</v>
-      </c>
-      <c r="J4" s="25" t="str">
+        <v>AUD/GBP  / EURO/AUD</v>
+      </c>
+      <c r="J4" s="24" t="str">
         <f>IF(H4="BAD","",CONCATENATE(B3,"/",B4))</f>
-        <v>GBP/USD</v>
-      </c>
-      <c r="K4" s="24">
+        <v/>
+      </c>
+      <c r="K4" s="23">
         <f>E3/F4</f>
-        <v>0.70882395697048994</v>
-      </c>
-      <c r="L4" s="26">
+        <v>2.068862987630828</v>
+      </c>
+      <c r="L4" s="25">
         <f>F3/E4</f>
-        <v>0.7110625909752547</v>
+        <v>2.068862987630828</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -929,238 +926,238 @@
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" s="8">
-        <v>113.33</v>
-      </c>
-      <c r="F5" s="9">
-        <v>114.22</v>
-      </c>
-      <c r="H5" s="27" t="str">
+      <c r="E5" s="7">
+        <v>1.4380999999999999</v>
+      </c>
+      <c r="F5" s="7">
+        <v>1.4380999999999999</v>
+      </c>
+      <c r="H5" s="26" t="str">
         <f>IF(D3&lt;&gt;D4,"BAD","OK")</f>
-        <v>OK</v>
-      </c>
-      <c r="I5" s="28" t="str">
+        <v>BAD</v>
+      </c>
+      <c r="I5" s="27" t="str">
         <f>CONCATENATE( B4, "/", D4, "  / ", B3, "/",D3)</f>
-        <v>USD/AUD  / GBP/AUD</v>
-      </c>
-      <c r="J5" s="31" t="str">
+        <v>EURO/AUD  / AUD/GBP</v>
+      </c>
+      <c r="J5" s="30" t="str">
         <f>IF(H5="BAD","",CONCATENATE(B4,"/",B3))</f>
-        <v>USD/GBP</v>
-      </c>
-      <c r="K5" s="28">
+        <v/>
+      </c>
+      <c r="K5" s="27">
         <f>E4/F3</f>
-        <v>1.4063459570112591</v>
-      </c>
-      <c r="L5" s="29">
+        <v>0.48335728657660243</v>
+      </c>
+      <c r="L5" s="28">
         <f>F4/E3</f>
-        <v>1.4107875307629203</v>
+        <v>0.48335728657660243</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H6" s="20" t="str">
+      <c r="H6" s="19" t="str">
         <f>IF(D3=D5,"BAD","OK")</f>
         <v>BAD</v>
       </c>
-      <c r="I6" s="21" t="str">
+      <c r="I6" s="20" t="str">
         <f>CONCATENATE(B3, "/",D3, " x ", B5, "/", D5 )</f>
-        <v>GBP/AUD x Yen/AUD</v>
-      </c>
-      <c r="J6" s="30" t="str">
+        <v>AUD/GBP x EURO/GBP</v>
+      </c>
+      <c r="J6" s="29" t="str">
         <f>IF(H6="BAD","",CONCATENATE(B3,"/",D5))</f>
         <v/>
       </c>
-      <c r="K6" s="21">
+      <c r="K6" s="20">
         <f>E3*E5</f>
-        <v>55.259707999999996</v>
-      </c>
-      <c r="L6" s="22">
+        <v>2.5015749499999997</v>
+      </c>
+      <c r="L6" s="21">
         <f>F3*F5</f>
-        <v>55.796469999999999</v>
+        <v>2.5015749499999997</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H7" s="23" t="str">
+      <c r="H7" s="22" t="str">
         <f>IF(D3&lt;&gt;D5,"BAD","OK")</f>
         <v>OK</v>
       </c>
-      <c r="I7" s="24" t="str">
+      <c r="I7" s="23" t="str">
         <f>CONCATENATE(B3, "/",D3, " / ", B5, "/", D5 )</f>
-        <v>GBP/AUD / Yen/AUD</v>
-      </c>
-      <c r="J7" s="25" t="str">
+        <v>AUD/GBP / EURO/GBP</v>
+      </c>
+      <c r="J7" s="24" t="str">
         <f>IF(H7="BAD","",CONCATENATE(B3,"/",B5))</f>
-        <v>GBP/Yen</v>
-      </c>
-      <c r="K7" s="24">
+        <v>AUD/EURO</v>
+      </c>
+      <c r="K7" s="23">
         <f>E3/F5</f>
-        <v>4.2689546489231307E-3</v>
-      </c>
-      <c r="L7" s="26">
+        <v>1.2095820874765317</v>
+      </c>
+      <c r="L7" s="25">
         <f>F3/E5</f>
-        <v>4.3104208947321978E-3</v>
-      </c>
-      <c r="M7" s="15"/>
+        <v>1.2095820874765317</v>
+      </c>
+      <c r="M7" s="14"/>
     </row>
     <row r="8" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H8" s="27" t="str">
+      <c r="H8" s="26" t="str">
         <f>IF(D3&lt;&gt;D5,"BAD","OK")</f>
         <v>OK</v>
       </c>
-      <c r="I8" s="28" t="str">
+      <c r="I8" s="27" t="str">
         <f>CONCATENATE(B5, "/", D5, " / ", B3, "/", D3)</f>
-        <v>Yen/AUD / GBP/AUD</v>
-      </c>
-      <c r="J8" s="31" t="str">
+        <v>EURO/GBP / AUD/GBP</v>
+      </c>
+      <c r="J8" s="30" t="str">
         <f>IF(H8="BAD","",CONCATENATE(B5,"/",B3))</f>
-        <v>Yen/GBP</v>
-      </c>
-      <c r="K8" s="28">
+        <v>EURO/AUD</v>
+      </c>
+      <c r="K8" s="27">
         <f>E5/F3</f>
-        <v>231.99590583418629</v>
-      </c>
-      <c r="L8" s="29">
+        <v>0.82673181948835861</v>
+      </c>
+      <c r="L8" s="28">
         <f>F5/E3</f>
-        <v>234.24938474159148</v>
-      </c>
-      <c r="M8" s="16"/>
+        <v>0.82673181948835861</v>
+      </c>
+      <c r="M8" s="15"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H9" s="20" t="str">
+      <c r="H9" s="19" t="str">
         <f>IF(D4=D5, "BAD", "OK")</f>
+        <v>OK</v>
+      </c>
+      <c r="I9" s="20" t="str">
+        <f>CONCATENATE(B4, "/", D4, " x ", B5, "/", D5)</f>
+        <v>EURO/AUD x EURO/GBP</v>
+      </c>
+      <c r="J9" s="29"/>
+      <c r="K9" s="20">
+        <f>E4*E5</f>
+        <v>1.20915448</v>
+      </c>
+      <c r="L9" s="21">
+        <f>F4*F5</f>
+        <v>1.20915448</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H10" s="22" t="str">
+        <f>IF(D4&lt;&gt;D5, "BAD", "OK")</f>
         <v>BAD</v>
       </c>
-      <c r="I9" s="21" t="str">
-        <f>CONCATENATE(B4, "/", D4, " x ", B5, "/", D5)</f>
-        <v>USD/AUD x Yen/AUD</v>
-      </c>
-      <c r="J9" s="30"/>
-      <c r="K9" s="21">
-        <f>E4*E5</f>
-        <v>77.857710000000012</v>
-      </c>
-      <c r="L9" s="22">
-        <f>F4*F5</f>
-        <v>78.571937999999989</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H10" s="23" t="str">
+      <c r="I10" s="23" t="str">
+        <f>CONCATENATE(B4, "/", D4, " / ", B5, "/", D5)</f>
+        <v>EURO/AUD / EURO/GBP</v>
+      </c>
+      <c r="J10" s="24" t="str">
+        <f>IF(H10="OK", CONCATENATE(B4, "/", B5), "")</f>
+        <v/>
+      </c>
+      <c r="K10" s="23">
+        <f>E4/F5</f>
+        <v>0.58466031569431887</v>
+      </c>
+      <c r="L10" s="25">
+        <f>F4/E5</f>
+        <v>0.58466031569431887</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H11" s="26" t="str">
         <f>IF(D4&lt;&gt;D5, "BAD", "OK")</f>
-        <v>OK</v>
-      </c>
-      <c r="I10" s="24" t="str">
-        <f>CONCATENATE(B4, "/", D4, " / ", B5, "/", D5)</f>
-        <v>USD/AUD / Yen/AUD</v>
-      </c>
-      <c r="J10" s="25" t="str">
-        <f>IF(H10="OK", CONCATENATE(B4, "/", B5))</f>
-        <v>USD/Yen</v>
-      </c>
-      <c r="K10" s="24">
-        <f>E4/F5</f>
-        <v>6.014708457362984E-3</v>
-      </c>
-      <c r="L10" s="26">
-        <f>F4/E5</f>
-        <v>6.0698844083649514E-3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H11" s="27" t="str">
-        <f>IF(D4&lt;&gt;D5, "BAD", "OK")</f>
-        <v>OK</v>
-      </c>
-      <c r="I11" s="28" t="str">
+        <v>BAD</v>
+      </c>
+      <c r="I11" s="27" t="str">
         <f>CONCATENATE(B5, "/", D5, " / ", B4, "/", D4)</f>
-        <v>Yen/AUD / USD/AUD</v>
-      </c>
-      <c r="J11" s="31" t="str">
-        <f>IF(H11="OK", CONCATENATE(B5, "/", B4))</f>
-        <v>Yen/USD</v>
-      </c>
-      <c r="K11" s="28">
+        <v>EURO/GBP / EURO/AUD</v>
+      </c>
+      <c r="J11" s="30" t="str">
+        <f>IF(H11="OK", CONCATENATE(B5, "/", B4), "")</f>
+        <v/>
+      </c>
+      <c r="K11" s="27">
         <f>E5*F4</f>
-        <v>77.959706999999995</v>
-      </c>
-      <c r="L11" s="29">
+        <v>1.20915448</v>
+      </c>
+      <c r="L11" s="28">
         <f>F5*E4</f>
-        <v>78.46914000000001</v>
+        <v>1.20915448</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D14" s="34" t="s">
+      <c r="D14" s="59" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="59"/>
+      <c r="F14" s="59"/>
+      <c r="G14" s="60"/>
+      <c r="H14" s="60"/>
+      <c r="I14" s="60"/>
+      <c r="J14" s="60"/>
+      <c r="K14" s="60"/>
+      <c r="L14" s="60"/>
+    </row>
+    <row r="15" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D15" s="32"/>
+      <c r="E15" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="F15" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="I15" s="32"/>
+      <c r="J15" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="K15" s="42" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D16" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="35">
+        <v>1.3431</v>
+      </c>
+      <c r="F16" s="36">
+        <v>1.3435999999999999</v>
+      </c>
+      <c r="I16" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="J16" s="35">
+        <v>0.75800000000000001</v>
+      </c>
+      <c r="K16" s="36">
+        <v>0.75900000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D17" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="34"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="33"/>
-      <c r="H14" s="33"/>
-      <c r="I14" s="33"/>
-      <c r="J14" s="33"/>
-      <c r="K14" s="33"/>
-      <c r="L14" s="33"/>
-    </row>
-    <row r="15" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D15" s="35"/>
-      <c r="E15" s="44" t="s">
-        <v>0</v>
-      </c>
-      <c r="F15" s="45" t="s">
-        <v>1</v>
-      </c>
-      <c r="I15" s="35"/>
-      <c r="J15" s="44" t="s">
-        <v>0</v>
-      </c>
-      <c r="K15" s="45" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D16" s="35" t="s">
-        <v>13</v>
-      </c>
-      <c r="E16" s="38">
-        <v>1.3431</v>
-      </c>
-      <c r="F16" s="39">
-        <v>1.3435999999999999</v>
-      </c>
-      <c r="I16" s="35" t="s">
-        <v>13</v>
-      </c>
-      <c r="J16" s="38">
-        <v>0.75800000000000001</v>
-      </c>
-      <c r="K16" s="39">
-        <v>0.75900000000000001</v>
-      </c>
-    </row>
-    <row r="17" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D17" s="37" t="s">
+      <c r="E17" s="7">
+        <v>1.3431999999999999</v>
+      </c>
+      <c r="F17" s="8">
+        <v>1.3442000000000001</v>
+      </c>
+      <c r="I17" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="E17" s="8">
-        <v>1.3431999999999999</v>
-      </c>
-      <c r="F17" s="9">
-        <v>1.3442000000000001</v>
-      </c>
-      <c r="I17" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="J17" s="8">
+      <c r="J17" s="7">
         <v>40</v>
       </c>
-      <c r="K17" s="9">
+      <c r="K17" s="8">
         <v>30</v>
       </c>
       <c r="L17" t="str">
@@ -1169,37 +1166,37 @@
       </c>
     </row>
     <row r="18" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D18" s="36"/>
-      <c r="E18" s="40"/>
-      <c r="F18" s="41"/>
-      <c r="I18" s="47"/>
-      <c r="J18" s="48"/>
-      <c r="K18" s="49"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="37"/>
+      <c r="F18" s="38"/>
+      <c r="I18" s="44"/>
+      <c r="J18" s="45"/>
+      <c r="K18" s="46"/>
     </row>
     <row r="19" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D19" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="E19" s="42">
+      <c r="D19" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" s="39">
         <f>(E17-E16)*10000</f>
         <v>0.99999999999988987</v>
       </c>
-      <c r="F19" s="43">
+      <c r="F19" s="40">
         <f>(F17-F16)*10000</f>
         <v>6.0000000000015596</v>
       </c>
-      <c r="I19" s="46" t="s">
-        <v>17</v>
-      </c>
-      <c r="J19" s="42">
+      <c r="I19" s="43" t="s">
+        <v>15</v>
+      </c>
+      <c r="J19" s="39">
         <f>IF(J17&lt;K17,J16+(J17-10000),J16-(J17/10000))</f>
         <v>0.754</v>
       </c>
-      <c r="K19" s="43">
+      <c r="K19" s="40">
         <f>IF(J17&lt;K17,K16+(K17-10000),K16-(K17/10000))</f>
         <v>0.75600000000000001</v>
       </c>
-      <c r="L19" s="15" t="str">
+      <c r="L19" s="14" t="str">
         <f>IF(J17&gt;K17, "DISCOUNT", "PREMIUM")</f>
         <v>DISCOUNT</v>
       </c>
@@ -1217,7 +1214,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
@@ -1230,249 +1227,249 @@
   <sheetData>
     <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="47"/>
+      <c r="B3" s="55" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="49" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="50">
+        <v>1</v>
+      </c>
+      <c r="B4" s="9"/>
+      <c r="C4" s="52" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="51"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="50"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="17"/>
+      <c r="F5" s="51"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="50"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="17"/>
+      <c r="F6" s="51"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="50">
+        <v>2</v>
+      </c>
+      <c r="B7" s="9"/>
+      <c r="C7" s="52" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="51"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="50"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="9"/>
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="50"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="9"/>
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="50">
+        <v>3</v>
+      </c>
+      <c r="B10" s="9"/>
+      <c r="C10" s="52" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="9"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="3"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="50">
+        <v>4</v>
+      </c>
+      <c r="B11" s="9"/>
+      <c r="C11" s="52" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="9"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="3"/>
+    </row>
+    <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="50"/>
+      <c r="B12" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="57"/>
+      <c r="F12" s="58"/>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="50"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="51"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="50"/>
+      <c r="B14" s="56" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="51"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="50"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="9"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="3"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="50"/>
+      <c r="B16" s="56" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="51"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="50">
+        <v>5</v>
+      </c>
+      <c r="B17" s="9"/>
+      <c r="C17" s="52" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="9"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="3"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="50">
+        <v>6</v>
+      </c>
+      <c r="B18" s="9"/>
+      <c r="C18" s="52" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="9"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="3"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="50">
+        <v>7</v>
+      </c>
+      <c r="B19" s="9"/>
+      <c r="C19" s="52" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" s="9"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="3"/>
+    </row>
+    <row r="20" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="50"/>
+      <c r="B20" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="57"/>
+      <c r="F20" s="58"/>
+    </row>
+    <row r="21" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="50"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="51"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="50">
+        <v>8</v>
+      </c>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D22" s="9"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="3"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="50"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="51"/>
+    </row>
+    <row r="24" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="53"/>
+      <c r="B24" s="54" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="50"/>
-      <c r="B3" s="58" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51" t="s">
-        <v>25</v>
-      </c>
-      <c r="F3" s="52" t="s">
-        <v>26</v>
-      </c>
-      <c r="G3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="53">
-        <v>1</v>
-      </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="55" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="54"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="53"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="18"/>
-      <c r="F5" s="54"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="53"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="18"/>
-      <c r="F6" s="54"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="53">
-        <v>2</v>
-      </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="55" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="54"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="53"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="10"/>
-      <c r="F8" s="3"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="53"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" s="10"/>
-      <c r="F9" s="3"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="53">
-        <v>3</v>
-      </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="55" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="3"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="53">
-        <v>4</v>
-      </c>
-      <c r="B11" s="10"/>
-      <c r="C11" s="55" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="10"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="3"/>
-    </row>
-    <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="53"/>
-      <c r="B12" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="60"/>
-      <c r="F12" s="61"/>
-    </row>
-    <row r="13" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="53"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="54"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="53"/>
-      <c r="B14" s="59" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="54"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="53"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="55" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" s="10"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="3"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="53"/>
-      <c r="B16" s="59" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="54"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="53">
-        <v>5</v>
-      </c>
-      <c r="B17" s="10"/>
-      <c r="C17" s="55" t="s">
-        <v>31</v>
-      </c>
-      <c r="D17" s="10"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="3"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="53">
-        <v>6</v>
-      </c>
-      <c r="B18" s="10"/>
-      <c r="C18" s="55" t="s">
-        <v>30</v>
-      </c>
-      <c r="D18" s="10"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="3"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="53">
-        <v>7</v>
-      </c>
-      <c r="B19" s="10"/>
-      <c r="C19" s="55" t="s">
-        <v>32</v>
-      </c>
-      <c r="D19" s="10"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="3"/>
-    </row>
-    <row r="20" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="53"/>
-      <c r="B20" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="60"/>
-      <c r="F20" s="61"/>
-    </row>
-    <row r="21" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="53"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="54"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="53">
-        <v>8</v>
-      </c>
-      <c r="B22" s="10"/>
-      <c r="C22" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D22" s="10"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="3"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="53"/>
-      <c r="B23" s="10"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="54"/>
-    </row>
-    <row r="24" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="56"/>
-      <c r="B24" s="57" t="s">
-        <v>37</v>
-      </c>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="19"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="18"/>
       <c r="F24" s="5"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>